<commit_message>
Fix sep=';'. Now all sep=','
</commit_message>
<xml_diff>
--- a/support_files/ExcelFile_default.xlsx
+++ b/support_files/ExcelFile_default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t xml:space="preserve">countries</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t xml:space="preserve">../Importation_Data/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw generation directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raw exchange directory</t>
   </si>
   <si>
     <t xml:space="preserve">saving directory</t>
@@ -228,15 +234,15 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -396,17 +402,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,23 +440,23 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="0" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>28</v>
       </c>
     </row>
@@ -462,6 +468,16 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix negative residual & add default Mapping
</commit_message>
<xml_diff>
--- a/support_files/ExcelFile_default.xlsx
+++ b/support_files/ExcelFile_default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t xml:space="preserve">countries</t>
   </si>
@@ -86,13 +86,13 @@
     <t xml:space="preserve">generation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../Generation_Data/</t>
+    <t xml:space="preserve">../Data_Generation/</t>
   </si>
   <si>
     <t xml:space="preserve">exchange directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../Importation_Data/</t>
+    <t xml:space="preserve">../Data_Exchanges/</t>
   </si>
   <si>
     <t xml:space="preserve">raw generation directory</t>
@@ -104,10 +104,13 @@
     <t xml:space="preserve">saving directory</t>
   </si>
   <si>
+    <t xml:space="preserve">saving generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saving exchanges</t>
+  </si>
+  <si>
     <t xml:space="preserve">mapping file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../Mappings/Mapping_ei_entsoe_v1_190204.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">neighboring file</t>
@@ -234,15 +237,15 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4948979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,17 +405,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,34 +453,38 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="0" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement Autom Cleaning Bypass
</commit_message>
<xml_diff>
--- a/support_files/ExcelFile_default.xlsx
+++ b/support_files/ExcelFile_default.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>countries</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>remove unused</t>
+  </si>
+  <si>
+    <t>data cleaning</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -195,15 +198,59 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,11 +531,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -524,7 +569,7 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -532,19 +577,19 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>2017</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -552,19 +597,19 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>2017</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>23</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
     </row>
@@ -572,7 +617,7 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -580,7 +625,7 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -588,7 +633,7 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="b">
+      <c r="B7" s="4" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -597,7 +642,7 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="b">
+      <c r="B8" s="4" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -606,7 +651,7 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="b">
+      <c r="B9" s="4" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -615,7 +660,7 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="b">
+      <c r="B10" s="4" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -624,7 +669,7 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="b">
+      <c r="B11" s="4" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -633,9 +678,17 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="b">
+      <c r="B12" s="4" t="b">
         <f>FALSE()</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +706,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -670,7 +723,7 @@
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -678,7 +731,7 @@
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -686,51 +739,61 @@
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B8" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -746,49 +809,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove savegen and saveimp parameters
</commit_message>
<xml_diff>
--- a/support_files/ExcelFile_default.xlsx
+++ b/support_files/ExcelFile_default.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">countries</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t xml:space="preserve">saving directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saving generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">saving exchanges</t>
   </si>
   <si>
     <t xml:space="preserve">FU vector</t>
@@ -159,7 +153,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;e&quot;AN&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -298,11 +292,11 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.15"/>
@@ -474,13 +468,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.15"/>
@@ -523,19 +517,19 @@
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B9" s="3"/>
+    </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
@@ -560,18 +554,8 @@
       </c>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="3"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -594,23 +578,23 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>22</v>
@@ -618,25 +602,25 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3"/>
     </row>

</xml_diff>